<commit_message>
feat: add icons, file generator
</commit_message>
<xml_diff>
--- a/assets/files/functional-specification.xlsx
+++ b/assets/files/functional-specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wonsik/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5D5D91-115B-854E-B99B-47299C0D1026}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEED922-ED80-C846-8119-6ED77270FF20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13680" yWindow="3060" windowWidth="24960" windowHeight="15140" xr2:uid="{981D4944-43AC-494B-9C10-61AD90DF9E4F}"/>
+    <workbookView xWindow="41220" yWindow="4480" windowWidth="15040" windowHeight="14540" activeTab="1" xr2:uid="{981D4944-43AC-494B-9C10-61AD90DF9E4F}"/>
   </bookViews>
   <sheets>
     <sheet name="level3" sheetId="3" r:id="rId1"/>
@@ -28,10 +28,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="155">
   <si>
-    <t>ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>WCM010101</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -588,14 +584,6 @@
   <si>
     <t>영업 이익 등 실적 정보 제공</t>
     <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>COMMENT</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LEVEL3_ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -713,6 +701,18 @@
   <si>
     <t>저장</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>level3Id</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1199,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77878D12-3F47-C245-BAE7-AFF9BCDF23AD}">
   <dimension ref="A1:B104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1213,724 +1213,724 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:2" ht="19">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" ht="76">
       <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" ht="19">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" ht="19">
       <c r="A7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" ht="19">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" ht="19">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" ht="19">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" ht="19">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" ht="38">
       <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19">
       <c r="A13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19">
       <c r="A14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19">
       <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19">
       <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19">
       <c r="A17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19">
       <c r="A18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19">
       <c r="A19" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" ht="19">
       <c r="A20" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="19">
       <c r="A21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19">
       <c r="A22" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="19">
       <c r="A23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="19">
       <c r="A24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="19">
       <c r="A25" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19">
       <c r="A26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19">
       <c r="A27" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="6"/>
     </row>
     <row r="28" spans="1:2" ht="19">
       <c r="A28" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="6"/>
     </row>
     <row r="29" spans="1:2" ht="19">
       <c r="A29" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="38">
       <c r="A30" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19">
       <c r="A31" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="6"/>
     </row>
     <row r="32" spans="1:2" ht="38">
       <c r="A32" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="19">
       <c r="A33" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19">
       <c r="A34" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="38">
       <c r="A35" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="19">
       <c r="A36" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="19">
       <c r="A37" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="19">
       <c r="A38" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="19">
       <c r="A39" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B39" s="6"/>
     </row>
     <row r="40" spans="1:2" ht="19">
       <c r="A40" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="19">
       <c r="A41" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41" s="6"/>
     </row>
     <row r="42" spans="1:2" ht="19">
       <c r="A42" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B42" s="6"/>
     </row>
     <row r="43" spans="1:2" ht="19">
       <c r="A43" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="19">
       <c r="A44" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="19">
       <c r="A45" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="19">
       <c r="A46" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="19">
       <c r="A47" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="19">
       <c r="A48" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B48" s="6"/>
     </row>
     <row r="49" spans="1:2" ht="19">
       <c r="A49" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B49" s="6"/>
     </row>
     <row r="50" spans="1:2" ht="19">
       <c r="A50" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B50" s="6"/>
     </row>
     <row r="51" spans="1:2" ht="19">
       <c r="A51" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="19">
       <c r="A52" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B52" s="6"/>
     </row>
     <row r="53" spans="1:2" ht="19">
       <c r="A53" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="38">
       <c r="A54" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="19">
       <c r="A55" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B55" s="6"/>
     </row>
     <row r="56" spans="1:2" ht="19">
       <c r="A56" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="19">
       <c r="A57" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B57" s="6"/>
     </row>
     <row r="58" spans="1:2" ht="19">
       <c r="A58" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="19">
       <c r="A59" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B59" s="6"/>
     </row>
     <row r="60" spans="1:2" ht="19">
       <c r="A60" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="19">
       <c r="A61" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="38">
       <c r="A62" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="19">
       <c r="A63" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B63" s="6"/>
     </row>
     <row r="64" spans="1:2" ht="19">
       <c r="A64" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B64" s="6"/>
     </row>
     <row r="65" spans="1:2" ht="19">
       <c r="A65" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B65" s="6"/>
     </row>
     <row r="66" spans="1:2" ht="38">
       <c r="A66" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="19">
       <c r="A67" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B67" s="6"/>
     </row>
     <row r="68" spans="1:2" ht="19">
       <c r="A68" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B68" s="6"/>
     </row>
     <row r="69" spans="1:2" ht="19">
       <c r="A69" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B69" s="6"/>
     </row>
     <row r="70" spans="1:2" ht="19">
       <c r="A70" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B70" s="6"/>
     </row>
     <row r="71" spans="1:2" ht="19">
       <c r="A71" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B71" s="6"/>
     </row>
     <row r="72" spans="1:2" ht="19">
       <c r="A72" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B72" s="6"/>
     </row>
     <row r="73" spans="1:2" ht="19">
       <c r="A73" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B73" s="6"/>
     </row>
     <row r="74" spans="1:2" ht="19">
       <c r="A74" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B74" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="38">
       <c r="A75" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B75" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="19">
       <c r="A76" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B76" s="7"/>
     </row>
     <row r="77" spans="1:2" ht="19">
       <c r="A77" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B77" s="6"/>
     </row>
     <row r="78" spans="1:2" ht="19">
       <c r="A78" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B78" s="6"/>
     </row>
     <row r="79" spans="1:2" ht="19">
       <c r="A79" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B79" s="6"/>
     </row>
     <row r="80" spans="1:2" ht="19">
       <c r="A80" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B80" s="6"/>
     </row>
     <row r="81" spans="1:2" ht="19">
       <c r="A81" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="38">
       <c r="A82" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B82" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="B82" s="7" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="19">
       <c r="A83" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B83" s="6"/>
     </row>
     <row r="84" spans="1:2" ht="19">
       <c r="A84" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B84" s="6"/>
     </row>
     <row r="85" spans="1:2" ht="19">
       <c r="A85" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B85" s="6"/>
     </row>
     <row r="86" spans="1:2" ht="19">
       <c r="A86" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B86" s="6"/>
     </row>
     <row r="87" spans="1:2" ht="19">
       <c r="A87" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B87" s="6"/>
     </row>
     <row r="88" spans="1:2" ht="19">
       <c r="A88" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="38">
       <c r="A89" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B89" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="19">
       <c r="A90" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B90" s="6"/>
     </row>
     <row r="91" spans="1:2" ht="19">
       <c r="A91" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B91" s="6"/>
     </row>
     <row r="92" spans="1:2" ht="19">
       <c r="A92" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B92" s="6"/>
     </row>
     <row r="93" spans="1:2" ht="19">
       <c r="A93" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B93" s="6"/>
     </row>
     <row r="94" spans="1:2" ht="19">
       <c r="A94" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="38">
       <c r="A95" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B95" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="19">
       <c r="A96" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B96" s="6"/>
     </row>
     <row r="97" spans="1:2" ht="19">
       <c r="A97" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B97" s="6"/>
     </row>
     <row r="98" spans="1:2" ht="19">
       <c r="A98" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B98" s="6"/>
     </row>
     <row r="99" spans="1:2" ht="19">
       <c r="A99" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B99" s="6"/>
     </row>
     <row r="100" spans="1:2" ht="19">
       <c r="A100" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B100" s="6"/>
     </row>
     <row r="101" spans="1:2" ht="19">
       <c r="A101" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B101" s="6"/>
     </row>
     <row r="102" spans="1:2" ht="19">
       <c r="A102" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B102" s="6"/>
     </row>
     <row r="103" spans="1:2" ht="19">
       <c r="A103" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B103" s="6"/>
     </row>
     <row r="104" spans="1:2" ht="19">
       <c r="A104" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B104" s="6" t="s">
         <v>145</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1944,7 +1944,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52195D5B-9850-6846-902E-1864C94604AB}">
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
@@ -1956,1157 +1958,1157 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19">
       <c r="A1" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="19">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="19">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="19">
       <c r="A13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="19">
       <c r="A14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19">
       <c r="A15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="19">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="19">
       <c r="A17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="19">
       <c r="A18" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="19">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="19">
       <c r="A20" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="19">
       <c r="A21" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="19">
       <c r="A22" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="19">
       <c r="A23" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="19">
       <c r="A24" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="19">
       <c r="A25" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="19">
       <c r="A26" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="19">
       <c r="A27" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="19">
       <c r="A28" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="19">
       <c r="A29" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="19">
       <c r="A30" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="19">
       <c r="A31" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="19">
       <c r="A32" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="19">
       <c r="A33" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="19">
       <c r="A34" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="19">
       <c r="A35" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="19">
       <c r="A36" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="19">
       <c r="A37" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="19">
       <c r="A38" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="19">
       <c r="A39" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="19">
       <c r="A40" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="19">
       <c r="A41" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="19">
       <c r="A42" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="19">
       <c r="A43" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="19">
       <c r="A44" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="19">
       <c r="A45" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="19">
       <c r="A46" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="19">
       <c r="A47" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="19">
       <c r="A48" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="19">
       <c r="A49" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="19">
       <c r="A50" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="19">
       <c r="A51" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="19">
       <c r="A52" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="19">
       <c r="A53" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="19">
       <c r="A54" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="19">
       <c r="A55" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="19">
       <c r="A56" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="19">
       <c r="A57" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="19">
       <c r="A58" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="19">
       <c r="A59" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="19">
       <c r="A60" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="19">
       <c r="A61" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="19">
       <c r="A62" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="19">
       <c r="A63" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="19">
       <c r="A64" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="19">
       <c r="A65" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="19">
       <c r="A66" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="19">
       <c r="A67" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="19">
       <c r="A68" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="19">
       <c r="A69" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="19">
       <c r="A70" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="19">
       <c r="A71" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="19">
       <c r="A72" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="19">
       <c r="A73" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="19">
       <c r="A74" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="19">
       <c r="A75" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="19">
       <c r="A76" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="19">
       <c r="A77" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="19">
       <c r="A78" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="19">
       <c r="A79" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="19">
       <c r="A80" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="19">
       <c r="A81" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="19">
       <c r="A82" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="19">
       <c r="A83" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="19">
       <c r="A84" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="19">
       <c r="A85" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="19">
       <c r="A86" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="19">
       <c r="A87" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="19">
       <c r="A88" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="19">
       <c r="A89" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="19">
       <c r="A90" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="19">
       <c r="A91" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="19">
       <c r="A92" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="19">
       <c r="A93" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="19">
       <c r="A94" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="19">
       <c r="A95" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="19">
       <c r="A96" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="19">
       <c r="A97" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="19">
       <c r="A98" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="19">
       <c r="A99" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="19">
       <c r="A100" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="19">
       <c r="A101" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="19">
       <c r="A102" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="19">
       <c r="A103" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="19">
       <c r="A104" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="19">
       <c r="A105" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>